<commit_message>
Added order customisation functionalities
</commit_message>
<xml_diff>
--- a/data/menu.xlsx
+++ b/data/menu.xlsx
@@ -1,19 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10608"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/anandbala/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/anandbala/Workspace/foodapp/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C96D8DD5-B11F-AD4A-A036-B2046E7BFDB2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{659BFC2F-1B85-9849-B86A-22CA41C4C324}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="740" windowWidth="30240" windowHeight="18900" xr2:uid="{4CD19E1D-1312-8640-97BE-438176FCA8FB}"/>
+    <workbookView xWindow="36000" yWindow="-5880" windowWidth="38400" windowHeight="21600" activeTab="1" xr2:uid="{4CD19E1D-1312-8640-97BE-438176FCA8FB}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="businesses" sheetId="4" r:id="rId1"/>
+    <sheet name="menu_items" sheetId="1" r:id="rId2"/>
+    <sheet name="customisation_groups" sheetId="2" r:id="rId3"/>
+    <sheet name="customisation_options" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -36,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="253" uniqueCount="48">
   <si>
     <t>title</t>
   </si>
@@ -47,34 +50,139 @@
     <t>price</t>
   </si>
   <si>
-    <t>ice milo</t>
-  </si>
-  <si>
-    <t>nice dirnk</t>
-  </si>
-  <si>
-    <t>sugarcane</t>
-  </si>
-  <si>
-    <t>refreshing</t>
-  </si>
-  <si>
-    <t>waffle</t>
-  </si>
-  <si>
-    <t>blueberry</t>
-  </si>
-  <si>
     <t>img</t>
   </si>
   <si>
-    <t>data:image/jpeg;base64,/9j/4AAQSkZJRgABAQAAAQABAAD/2wCEAAkGBwgHBgkIBwgKCgkLDRYPDQwMDRsUFRAWIB0iIiAdHx8kKDQsJCYxJx8fLT0tMTU3Ojo6Iys/RD84QzQ5OjcBCgoKDQwNGg8PGjclHyU3Nzc3Nzc3Nzc3Nzc3Nzc3Nzc3Nzc3Nzc3Nzc3Nzc3Nzc3Nzc3Nzc3Nzc3Nzc3Nzc3N//AABEIAJQAlQMBIgACEQEDEQH/xAAcAAABBQEBAQAAAAAAAAAAAAAAAgMEBQYBBwj/xAA+EAABAwIEBAQCBQkJAAAAAAABAAIDBBEFEiExBhNBUSIyYXEHkVJigaGxFCQzQlOSk8HRFSNDVHJzgrLh/8QAGQEAAgMBAAAAAAAAAAAAAAAAAAMBAgQF/8QAIBEBAAIDAAIDAQEAAAAAAAAAAAECAxExEiEEMlEiQf/aAAwDAQACEQMRAD8A8NQhCAEISmi6AG7hSgzw3TBYQb2UqIgx2O6AivCb6p94T+G4ZV4rWMpaCB00z9mt/EnogIKWzQrTYjwDxJh8fMmw4vjDS4uge1+UDvYqnw7BsQxKV0eH0c9Q9mrgxmyNwt4z+CndcgKwj2CHcN43RvvU4XVx2+lGptHhWI1TiyChqHvaLkCM6fNHlH6nwt+I4CQ9qfLHMc5kgyuabEHcHskuCshV1Dd1XS+ZW9U3dVU3mUKmUpu6SlN3UB2y6uoUoNIQhQkJyLdNpyPfVATYWtkIGp9lIno5GtDoopPsYStz8OpZselmoqt7vzeEPYWP5Yy3sQbe4WjxKkwjDpuTW1sXPcMwjlq3AAd9Cl3yeM6Ophm8beaYBwvVYrLnqYpIqVupJsx0n1W32PqQV6lQsh4dwKSow7BKJssLC6RgkF5rdA4gkm34JNNhdLI6WGow6KOVrgGGWqcWuv1Nj+CaxbhnEGOD4qOjytcMojebAepJ16pM5oaa4NQbi4ypMXpG0RwyqojM/KSG6AnTp0+wK8pOHJMPkbBRzRQi13ujdqSd1l6bBq19fK+SCOmbGW8u7rh5sTc67LZOxLDKODPPC0SmwtTEuuba7qlr1kylLVT6fB2uYS+pfN2cXC5UHiCAQOYaclr3AeU9lLjq6eOmZMIHvMhu1ltQPVSZYG1rc1Ox8LraZholxMTPqV/6jsPLeI+Fq+ev/LKKMSMnGZ4JDcrvt7qhnwTEonZX0jgR2cCvZ6nDsSy5BI131mOdf5KjquHq+bR7wJN8hPTve91ormmPRFsNZ9vIavC65oOajm3sCGk6/Ys/WRvilMcrCx7dC1wsQvaazhDF3Pc+NttNMklr/evL+KaqcV09DKCDE7K/mWc649bJtMnmzZcXgzqU3dcO6G7hMJOIXShSgyhCFCQE9ELplPweYIDScNzPpZ5Cxzm82F0dwftH3hW3EDqYYNFUPPMmlMjGuygmwPX8FSUQsARp2S6856FjcxzxPOnodVny493izZhyapMJmC4jO/Cq2N0zzIA0suTcWTVNjOKOcGGsmte2jyqihndBObbHQgdQnWyTc9zI3hrc1wCLpc4Y3MmRntqGzw/8pqLc6omcPVxV7SUcET2c3P4jYHMVksI/LzbLUMaP9taaNmLOZaGqgLvrx6JM0rvTVW8621tLStzNDi8gbeIq4gZkADXPsB9MrNYd/aphYKiqh5lvFki0VxTtretUz+El+OpXmdwuGtdmvnd+8iZgLg8l2YC179FEYKr/ADDf4a6DUEn84aSNxkGisXMaJqS5rXAOk013XzVxDM6pxitmeS5z53m5662X0FxHV1FDhFZWc5pMMLpACzcgaL5zqnFzyXeY6n3Wr40dlj+XPIQ11vmCCus8wWpiOkISkKUIyEIUJAT8HmCYCfh3CIDQ0XkCbrHsaXAuF0qid4UqsyjcbhRc2kq2HKZtXtA73UqIt555bmHXvuFFjLRUtJtl6hSXRxOqxZoA0NgEu3DKz7a3Cnx+Hxt+a1lA6N1vG0/8lisLo6Z9i6FpPey1WH0FJYHkM+SxX66OPbUUpZcWcPmrSAt7hUVJRU4taJoVrBT07bf3bUva8rJmXuPmkmGASOlblEjh4jfewTbIIh/ht+SUYo/oN+SmJU0yvxJqGQ8I1wztzSBsYF97uH8rrwaq82u69k+Lb2R4NSxBrbvqb7dmn+q8bqfMt3x4/hz/AJU7uiFdZ5gkpTPME9lPoXUKUIqEIUJAT0W4TQTkaAvKJ2icrtQx3oolK+wUqY5qYHsouZRXhud1m6XUzKWVLGno0a91Gg/SFTmMMtYwDe34Jc8Mr1o8J6LW4d5QslhFjYhaygNmhYrulj4v6X9VWULG5s36yrKU7KyiOhSjJTGlBK4zZcfoLqVHmfxim8WGwjs99vkF5TU7r0X4vz5sepYv2dPe3uf/ABeczldPFGqQ5Wed3lESmeYJKUzzBXJSSEIuhWRtEQuosqpcS4zqk2S2A3QE+ndspwdmpnehVZEbKbCS6nkaN8wKi3F6dNQnLN6HRS+cHTMLDYt0JVeSQ9OU7SJs19HKk8MifbYYM4+HstZQm4CyGCm1lraArDd0sfGgpToFZQlVdIdArOIpRsprXeFN1LWzROjkJDXWvbfddbe10iUmxsrKS8T+KNRzeL5xf9HDG37r/wA1jJTdaDjmbncXYq6+gmy/IALOvK6lPrDkZJ/qTK63cLi6N1JaShJuLIU7RoyurgXVCXQEtoSAli6AeYplKfBKPQFQG3Uukvnd6tUTxavTbz405AfG1NSeYpUbc1hcj2VJ4bHWtwg+Va2hOgWNwd2UNaSSAtfh7gWhYruhi40NHewKtogbKmpXWboVaRSHa6Semh2gCQ8pIeNE1UyCOGR52a0u+QU19yrPHzvjcpnxmvmvfmVMjh+8VXuTpObxE3J1JTTgurDi27JuyF1cUqu5ihcQgBKCQugoB0JxoCYBSw5ASWsHdPwANfp2KiMd6hSInOzi2VErR01L5ylQnxD3SZj4j0912E+IKn+Gx1qcHPlJ7LV0srYmZ3kNY0ak9FkcH1stdQtD2ZXAEO0IPVYsnW/FxoaU3aCNirKEa6qmoPyltTyy1hpw3wvvqD2IV1HpqEmY0fE7g/fsq/iObkYHiEt7FtPJ/wBSpvMjb5ntb7lZvj+vZFwxW8vM4yARgjbU2Vsf2UyTqsvEzGQ23ZNO0UkvvqmXWPQLpuPMGSkpx1uyQVKriEIQCUIQgO3Sg5JCEAvOnIpPG33TC6DYg9QgQmSnxFEbA5wum3uub9CF2M6hUN/1osKw2OSxJePZxWsw/CogB45hr+1cshhMzwRbZa/Dqh+UaOWPJvbfh00VHh0Yt4pj7yuVvFQU9hnaT/qeSqiinc4jQq1bIbDQpDUlNp6aPyRsHsFj/ifUNbw7kFvFM0LTPlNtdvdeffE2uikp6WkY8GQyF5b2A0TMHu8E551SXn7nDrZNktXXNTbguk5MuOt0SCum4SChDt0JKEICEIQHQghCEBwoQhCUm+eJoPTROZGtiLhuEIVV4OUlZLGRlt8lfUWL1TWXGTT0P9UISMkNeKVnR8S1/MDMsNgPon+qs6fiHEJpOWZGMH1WIQs1+tePjV0OGMqY2yVNTUy3F8pks37gFgPiWxkWM08ETGsjjgOUNHqhCv8AH+xXyfqxjk2R0Qhb3MkgpshCEIJQhCA//9k=</t>
-  </si>
-  <si>
-    <t>data:image/jpeg;base64,/9j/4AAQSkZJRgABAQAAAQABAAD/2wCEAAkGBwgHBgkIBwgKCgkLDRYPDQwMDRsUFRAWIB0iIiAdHx8kKDQsJCYxJx8fLT0tMTU3Ojo6Iys/RD84QzQ5OjcBCgoKDQwNGg8PGjclHyU3Nzc3Nzc3Nzc3Nzc3Nzc3Nzc3Nzc3Nzc3Nzc3Nzc3Nzc3Nzc3Nzc3Nzc3Nzc3Nzc3N//AABEIAJQAxAMBIgACEQEDEQH/xAAcAAACAwEBAQEAAAAAAAAAAAAFBgMEBwABAgj/xABAEAABAwMCBAMFBQcCBQUAAAABAgMEAAURBiESMUFREyJhBxRxgZEVIzKhsUJSYsHR4fBDciUzgrLxFiQ0otL/xAAaAQACAwEBAAAAAAAAAAAAAAACAwEEBQAG/8QALxEAAgIBBAIAAwcEAwAAAAAAAAECAxEEEiExE0EiUWEjcYGRwfDxFDKhsQUzQv/aAAwDAQACEQMRAD8ACWBhqRAWrxQhRUEtc9jgknb0xudqrMJT7+eE4C3Poev86ao/s8u9scAst3gyGUlRR4xU04nOM8gR07iryNBvhKXZciCy5xhSwXsp+QxWbZVLrBtVamC5yLtwdft01LHElxA3HYqwMj5Zpl000p2A7dNQ5Tb2jlhKgB4p7JHM9qsvR9P254PuKNzkDdLSBwMpP8/huKA3y6S7q/xyl+RGzbSdkIHoP50mGmjXLcTdrd8NsPzKN8ub11uLkt7bOyEDkhHQCli9v+QMg5zROc8hhsqUcdvWlh5xUmQSTsDmrleW8mbPhYJYg8Mpwccs0z2yQFlPbPVWN8Urt5SabNL2eRKCJEg+BDTnzEZUv/aO3rVgQw/Ckl1YZba4nCPKEjiOe2KZolueDaVzXERx2Xur6VRiOtQm/Dt7QZ4tlOc1q+JqUFa8KdWTk4yaHciMBNKreyAAHH1DueEflUzc9I/5UVpHxTmqrUfvyq43HA6VOWdgmE58DIwMb7Cl683syGEPe+vQ4yVEs3KKrxG0nkQ8noOnmGOe6TRybB97iLZS89HUrBS6wrC0EHII7/A7HkaR7m7JtU9KLy6LbOf8rN1jt5iTP4X2zslWP7GiJUUwj/6yk2cob1ZBjmMs4bukNviYX24gMlJ/KmyFIt1zjh6I6lTawClbS+IGszcddgy/cm2o9ulPjJt7547fOHdpX7B9MDnyoPHRKt9wWvSLj1suLeTJsctWQv1bzsofP59KnJ202V6C7wktKDuOWNjVMyFod4FoOfXpQPRntEg3p1MC4p+z7olXB4TmyVq7AncH0NO7rLUhOHmwr16/Wp4YDyuwQXVAbHny2r1K1AcQwO+BmvmbBfhhTjOXWMbgDKk/Kh4lYQOEglR6n9a4kKpV5d981GThYOcdqgYdLgwTg/lVlAGxO+Kg49QSEJ4wAalcRhAX0614VJJTk7V4eIrI4vL6VxxF5TvsPrXV7xY2/ma6uOEy7Myve3FOzEyFg78vyGdq+WMLRjKcj1qvfWokaMG4yAgDfjG6lHuT1NLbbU4r423/ACqPlB3pGGWOBqf4NyVj45oDc7iyxxJTgn1NfL0K4ONkGUkHP7m/60LkWOStPE8pSzz35VHjz2dvwB50pyWvHSo2meDbqaKG1Kb3wNqb9MadaYbauU5HnI4mG1f95/l/4piSSFttlLT2mA22iXdWyVbKbjqH5q/pTUlorUMjl9KsBBWcmrLLG9A8tg9ETEf0q+hhPh+ZIIG+/Q96jkvs29pLj6SQrlgV4NRWhuKXlyAM4AaI8yj2xUOytNxb5DjXOeGkQwFwzL8KPKcEleACobE9sUSfuSYS/CeZJWBlRSdqWbDcTJkvzYFrd4nCr3dLqRhIz3zt070XRb5c8rk3qQkNKAHhIGwGPw9+pFZX9XKEMQfxZ/Av/wBKs/adf5Cjd4jvL8OGlb7uN0p5D4n5VRv8STMt7zL/AALbdTgxlNpUgj59aWNQa7t+nvFg2phKX2vLx8OcDnzoRYHdW3e6xbw9HfXbgvIK1BHGD1Cc7ipc9RbHc3hfl/IcdPXD6ff2LXvk21Jk2yTHE+1IWfEgPgktDujqnHp/erbjseXbEueI7drKz/qZxNtfY5/aSO/LbpTfr20HjRqG3gEtJAebTzIB3+eP0oG5p16Uw3qXRToakhPiOxkcnBjfA5E908jWlpbfLD7ipdFRlnBReh/bHhInlm5NFvii3ZkhLikpOCh5J7DvuO5pu0XrR9l8W+5hxcQp4o7ygpS0NDYKUrqk468vhSnpxgz0uqMUIjuvlJixU8Jfd5+EgdAOauwrW9L6VatUF964pQ5OmjD/AA7pQCMBtP8ACBtRJtyyTOMVDDD6CCkFByO4oJerGHuKTCBS7zU2OS/h60J9l93cn6ejokrK3WUhtRVz2FOg2PKrXaKPTEKHMWjyuDCs4IPOisdwOAhKvjUmqrKVJVcYIIfQn71tI/5g7/Gl+13EHBzzqCRnC0pb3O/KvpJyVDOTmqTb3ijjTvjnVlpeAF5ByOdQcfZSrodq6vc46E11ccZRHWZ5Sog4X0HIU226Cx7oUgJ40qGM9Qd8Z+NBNKRS/GTsRt5cjnTxEhtMxQ2oBRJ54oEg5MEmElO/ASFc+I7Gq78NSkEY25bCmJTJSnOMp/zeoHIpKuJCiOLfFTgHIv2yxtrkOOyRiKzhah0Ueifn1q+4pUxwqVsDyA6VcvS0xwiAz+z5ncdVGo4DNC+8HZJWGNhgVfZYxvivWkJQMqIA7mq1w8acgR4LyPDP/MUDuR2/zn+q7LI1LLDrg5s+bnItLzK48iY0VoyQhpxKlg4xsnrS9GsA4kynSEp4vu23WRlQ9RuAauSXbbp5lyTLdCllR8Fvnwn/AD9KCab1ZIvuolMJ4VNhJUkrAzn+m9YeotndmajjBr0VOuPwsu3nWEGzJ9zirSXUJ4HF4wQeyRQ/SGtH7jqBMKUC3GSjgS2o75HU0q+0awSLXPE8AIbkrJIQrPCr+9B9JwZ9zv0ONaziUpfGFKJwnG5UT25/HlVmrTVzp3J8jXtz9Pma/cNDQ7pqiNdcIQ23946MAhagPKCPz+VDNX66RabrHgwylTCV/fdSQO1HdV3KXbLKuNbUrfdSAhWOayRuaw95Ulc112Uo8Sj584P17fCg06V3DfEeP39BcI5eX+BtirZB1PATKt0tbSnE7qQrc+ih1+Bpfs8STo27LYm+WNIXkODZsHPfpnPI/KofZdCmPoeLby246FjgUnnxY3Hwxina/Src2huDcnUH3nyJSoZ4j8K6Nzom8AX1LPj7X+iwzHSmQbnbAz47qMKCt0OA79ORPcfPNcm8z35raLnaywyj/UZe8UZ9RgGldDdx0olT1uC59mzlUfJLjXfgPUehpps13g3qImTBcDiDjiB/En0I6VsVWV3LjszbITqfzQK+z0aevy5cFXFbLgrxPKc8Dh5j4Hn9R0pxjvJdQCk5pP1XaZ64xlWRz79vCnYhPkfx2/dV69fzqhpHWsaZK+zpZLMrOG1L2Dp/dPZY5Y64+VNjJxe2QEoqUd0fxNHyDtzGazrV9s+x7micyMRJC/Nw/sL54+B3p+ZfC+Ywe1RXq2tXW1vw3gClxPPseh+Ro+xIiQZgd2Svc9qLxnlnYgEUiQ3nYMtyNJbV4jLhbWE9CDTjAk5GSjynGO9AEF08ShzH1rqqoyBsOL1FeVJwI0XFR9kMOJAXlIOfT5U0oQQnAAxmlD2byyIT9vfP30N1TROeYHI05cJzz+NQiXwzsZSU9x0r4ZbShzxXPwMp4zn05fnUoHDj0qrfXPd7Q5w7F5YTn0FSQLinvGecfdUNyVFR6CobZeZNymliyQxIjtnDktaylGf4dt6kXAE23SYx/wBVpSPqKIaJYchWFuEW225DSil5P8W2/wAMb1S1Vkq4rHstaeEXlvkvyi1AjF67yglHDnwmzjPxpahajbv/ALzEgAssMJxws7cfECPyODSNriRepV7cjXCUluM46fDJVhHBk4O3M4r60c+7aZCn2EKWlZAUpKc5AIOfpWdZVur355NOqpLj+Abqu0y7dPzILvhndrxDntkego77M7TPmy/eILKvDbykukEJSc9Vcj+taLdNPwdUyYrUtCgwyfFcGSkrTj8IxvzI7U2RWY8WM2xDYbYZQOFDbaQAkegqxTi6jbMVdqnB8LkXr/pn7XtL7E10cfhnAaT+1jYgmhlhgRtG6XU/ISlqS6guOZwFcuRPf/xTdMk+CkkkenrWNe0m5XOTNVEU26iMkjBxso0majGXir4Ip8lixJ8BnTermrm89GmhKFqcIbWeQQeWf8617qjSAuDhfgqAm80qSdl7cqRLK002SkxnJEt5QS0lKyBg8+RyT8dh1rUdMw51ujlVxkurWpGEtqAPCcbkqGwFVrqFTNTrlguLhblwWrY2jTOmElS0JcbQVONrVsFnc7/GscveoXrvehMWrCUuEoQTtjPStKuXumpmpNvTKC0JX5nEKxy5fHFZ9cbK/YW5TKmlrW8UeG8kA4Azkb8s5HL92naScJSfk4Ytxn2u2anpvUUa5WhKCQ4QngcSgZP0oVeIL9okquVifWw7w5cQ4nKFA74I+NXNEWxNmtJMvHGVca8nnkbD5D880r611wv7VRHg8Phtqw6ABuBtikw8nlxU+v8ARzhBNrHHsddNawiXRXuskCFcQMe7uK2X/sPXr60L1/oZN5Su52dtIuIGXWsYEgAfkrlg9eVDmLbF1Vby5HAakt+ZtWcKT6VeteqJdglN2fVYWDj7qcfwrT04v0z9e9a+n1iuW2awzOv0vjl9mC9F+0N2IUQNQrUW0nhEtzIW0RtwuA7/APV061r8KSiS2hbakqQoZCkHII9DWda50ai9oN2tCUC5BIK0A4TKT+nFjkevI0k6V1dP0w5wJSt+3BRDkRX42lZ34M8j/CdvhVxSceGVnBTWY9jb7UIIt98YnoyG5aSFYG3GnH6g/lXzZZ4WhtBI4epA5US1tc7fqnQblytT6XfdHEukYwpG+CkjocUg2aXwuJAVgHG1ExSNRYcPhjyprqGRJALCfOPoK8rjhWs812364lodSltUgpUtGc8KsDr8q1SM4Vtg7bCsTuE5D2uZEhpSVIS9hKk8jitgsz5djoJxgjY4oYjLFyEkp4qE6tVhENgdElRFGm0gjY79jQPVWTPjg9GhUvoWRW9GEp71dchoCvekDzlPC7j9tI6H61Vgg7UcjpyMHf40qypWwcWHCbhLKFPV2nIt4t5djBJW0AUpSMeXHL9D8qtWrT0G0WsKCFF3hSp0+ISVY3wfTO+KNKYQ0+eAgp/d796TfaHcZVtj8BedRDUFqLbafM6rtxfsjGPX4AE1i+Ocm4fwakbG0lngnl6ljMXaN7pKzMQTxMlXl4dspJ7HpTPDuj8qWhhuI6lCklTjp/C1jmPU/Cvz7p+FPud7jRoYW5IcdCiArYJHMk9ABW56gmO2qwOs2xCn3hkYRvg9h8Kl1y0+MS4/UbdCLailyLmutbfZ8ttqEEqUhwcauyev170xxnbXqe04AQtCkZUk/iScVhcp9x+U6uW0XJalnZ0YSj5cifSnD2fxZEuHJDKZCHgsJacQcJSeZJ6bDO3qOW9HOjZDc3z7C8axiPGBr0/poWm9vHPFGUjKV9Qdsig3tI1GIjfucZXBJVxJWAdkp5D65ppuN5iWsNe/ujhyG0uE44ldaUb7otV9ui5NocQ6tW/A4vyqHxNVKdkrFvCbk/ifpCloJuddbz7rCcSlbn4uMnhx136Vpj+nbg667GmNmSvh8jiPwLHp2PoaGaSsd1tF5VEcgKbbACo6ENhTaV9VF3mdiefQ4xWptgwogDjpccA87h24jWpbpK9Q89fUqy1llPWGZJq+5yIlrfgIirbmtpSME+YI7n5frWUICy6pTxPFnOFDma172mSIzjsaaNnm1hpZIzlB5fQ0EesMa7pMiLhD6D+0cJc67Gq8Jw0uV2n7LEV54JhT2fWaR4TM1DzralglJBA2/pTHqR21SQ1arwuMpLqwlvjODx9cdv71WTeI+nbU4tQ+5QAUK2545fCsevV4mX27rnqURg/dpHJIpNNc75uWcI67tZNasUhzTU5iwyx4kJ3iVFlLWck5zwHp+ldrzRpuzarvZ2/+IpGXmkjAkDv/ALx078qXdOX83hluDfY77oSQG3EoJIPSnTTN7CLxLs77xWWcFkufiKeoPU4JFaOmvbl4rFyUNTS4PyRMUbdebLy4Ti2VuILT7fLjTyKVD/MVascxKX0tOcKHOgV1+Fah7SNCe/odvtjbCJiUlcpgcnwN+JP8X6/GsfWlqUgKGQrntz+NXHmIjixZXZqVvkYjAK4yc74FeVncbUNxhtBlTaHuHktalA4+Ve0W5CvHIPaxt0e06vWmJgMyG0SEADCfMSDj5pNaPpKYl6C0jKfw4zmkL2mF96daJK0ZJjLGQnHlCyRt86v6IuQCQ1xYHQ88UMWMtiaq0c8qFambzKjqHItgVZZfUAOLmeY7V8XlHjQYzyTkJUQT86P0IKUZrxAkcak4IJ4etH445YoNBHI+lF2lpSkFRwDUxOAdzluwLt4islsnl0IqDXltF5tUR5ALoacDgZBx4npmvvVsd9Sws7oxt6VBpa5BzigSzkoGW89jivMb513zgvnlGxCO6uNi7QLs0KFoXTxWtSFXOS1xPPdh+6D0SPz50M0brNmfdXYl0UkIWrLS8fkai9rdxQ8pq3x91NkF5aBkJHak/SNtRPvcjxgpuKhs+CoK4fvBjh33xnercalbF22Pn0NwtqTXLNd1JpWFeGS7HbQHiPKpIGFehqww2xp/TIVwoZ8BsHAPLHMfOpLLCkRYAcW6pxCk+VBV+Ghdwk23U0aTaEPlbgIDiQcKRVPdlfv8yOf7c5SMd1lfnLzcnHBhLIUfDSFZx60e0Fqp6LNYQ5xuhKvKBkkfDHTvVDUuhZlnddWOFUZPJzOxPb4kU1+zbSIg+BdrjniXnwm0cgnqSfWtOaoen+HpExck230a9HkB5luQ0CEuJCgDsaqXOUQwsEZ2J2pFuHtMhWe6KiOMqkRd8OM4PCrt6irzXtA0vPhqcMtbbg2LCmlcZ+AHP5VCdrhuj7M+VWJYwIus56Zc5iA0h11xxzAS2AVHfOwO1N1rszdts6C+4pKXRxJOykpVtuPj+Ypfs8UT9YmYtgtRS2UtA7q4cjI9CobegJqX2kaqwyLRBRwSjsskY4E+nb+1Js+1Uao9vsuwTq76IJcNnU7UiLEuDa0oUSopySVD0P60nyrJNtElDT6FBsnAXjA370Otdyctk9D8BS/Lsog44x1+ArYrPKg3e0IfnRilK28nxE7KHcEdf7V1qs0nC5iOUlYtzRHpaE1ZLaufJcTlvBUr934UvWCY7N1Q/c0IHmJ3P7Kc9PUnevdYXtMnFphBQYSricP76qM6QtPhNtN8OFq87n8hVrQ1S/7JGdrL1J7UaQh//hbriuXgkk/KvzBwlzLrIPPPCOvwr9Gauki16Huz+cKTDWEf7iMD8zX55t6cJG+ccq0pdFCDafB4h1C05IJPXArqKC1MvjxFtKJPVJIzXUraWVaaFf46V66sKZD5fS6h3fGBkEbAfSmG8aThlXvUEe7SeRKE+VXxHel+8MF72lWWGFoLrSFvL4dgAo7f9v5itMKUqGMfh/WoiMsxhCigvxij3rPnwlSiD07UWYWmbCkspPmSONPyO9QXiGt0BAzhShw4OAMHIBPrmqTC1Wm4pcQ6Vxv9UHklJ2OD2GaJS9CZV+0WohCM5OMczRaKsKAwPL0PQ1Qfj+DKUkHCScpxvkVcYV07U1CCeZETNj+ETg78J50g3O3vQJiHW04cbVnHT5+laI2raoJ9uYnt5UOFwj8WM5+IrO12i83x1/3L/Jb0uq8TxLoT49vhz4ypKE8TEk/eZGeBXrX3ZNINWq++9NABlxshaTtwH+n6VYgMO2ma/EXwLjOklXC4CE59OfeqGoNRJsT7EWYqQGFgpD+AQjfbPpWOuPhxz8jR3zb4fDIfaZqcWaEuDbVkSHEYKUn8Ce/oKx+HdlQri1JgBSAgDi4ju6epNaHq7SbN1Si5NSVl54gqUpflUMchWfRbJJfu7dvZQVOOOBtHEMbk9e1aOllTKuS9+0dGtprHRr+nborUtpUl2MAEt8RWRlChk5Cj32NDL5dZkCyGPb2iW20FCGgOQ7/53o+qPB0Xo5xsvE8KSpbnLxFdqyyFq6Q7OdFzGWHDgFKd0DNU5USlNyqWUu/r9Blc4ZefwFB5b7rhCyeIq4qIWGHKmT2GY2StSwfRPqab7hp2BeleNaFZCsni/tRiyW236Wszk58+JcFNnicH4EDqBv8An+lX562DrxHv5AQo2S3MKKuUGxSmUy5aQ2PusnmvbnilTW+nUTprtzhSCpT5ypJOc7ch9KSrzcnLnMU8pRIySjJ3AzTHp+9SkxUJUkSAhfBwDPGMjY4xjHzzVeOltoirIPn2FGcLZOLIdIaXk3O7BlSeBpo5dJ3JHYfH/DTxrm6sWqM3Z7cEhfNQSc4Pr8KpPS12oiQ0nwHlIyrAwQME0vWxp/UN1ckv5UCskqP7vamUqWrmpSXCE6qapWEwlpWzOuKaedBXg54lDdR7/Wtb0/bvCQFKAyedB9OW1JwrhwgbJT2p1is8KU7YxW0lgxW8sz/223ERtNx7ek/eTHR5f4E7k/XArIIjfAgZG9MntPvIvmsHkML4mIP/ALZvHLOfP+e3yocy2EFCAnfGM4zQyCRfiNr8BPkz65FdReKwCynlXUBIJj6oM/XzF/cZ8BsLSkNA5w3uNz1O+a3ZhwOx/EQfIrdJ7ivzRFWfevG4UpKlcXCkbDO+BW7aauinNOs8A++JShGeWScDPw549KXF84NG+C2poMOPJL6YjZCniOJWU8QaT3Pqeg/oaTrvqKLAuXuTV8tSl5U3IakZSUnPcbf9JxRHXmoTo6xpchIQuZIc8Nkr3yrBKlq7kf0rBJD7sqS5IkLUt51RWtZ5qJ5mpYqCP0TbpImRSwp2O48wAW1MryHGuhxkkY5denerrJGTuNtq/Pul7vJsF2Znw/2VAOtY2dR1Sfl16VvtvlxbnAZuNvcC4zwyD1B6g9iOVNg8oq3V7XlBFs7YqUlQaWU5/D051XbNTcRGMDNE1lCk+RScbnT7nwMoXzAV0S2PU/y6186hsC73bFRJa2w82cE4zg/3p0ThI8oAzS9qdM23vfakFtL7BTwyo5VwkgfhUn16EfDtWNP/AI5Uwc4tt9s0atVKySjjHyMqsULUMO5yrMzHclRWjhTK9kAHso/hp2ahxYs1M1DLZfZ6ggqRkbk458udDHNS3BUhxcCJKQXBhSSxkn4mli6uXxcoTZ81cUpOEIbUkuHttyA/zeqco+d56ZofFBPK4IfaZNmzpwabaUILYBCwchR6n0pFSy4Fbn552rb7A25cbZ/xOI2sH9xPP1x/SqiNEWpi9x57SUqjfjUwpWAFDcHHMjPMVbqvenj47I4/UTF12SyiL2eWNUPTb864caQ6SW0rOAEd/nvVO7yrVf4EqAw/uyoZIzjPp6b1L7UNV+Ez9mRHPOoAFKMeUb86zG3yJEOR4rClFeMqA6ilx0zubvXD9Bq3a8SL14069anFAAuN4B48cv6VoWg7NA0/bnLrdkJW8tAU1ncA9Ejua902+9cLY4ZcBYShBwtY2VS9qCc9Jf8As9g+G0jAShsfh9M1MLrr34WvvZFyhVFsF6mvDt5uz6Y+zal4UQc8R/pyrQtKWH3eKzHSkhXCC4QOZpf0ppNYuTAcb/5aipav2SMZT887VsNtgIYQAAM1q6atQWEujJvscn2TW6IGUDahPtE1IjTGm3Hm1D3yQfBjIB34iD5vgBk0xPPMQYrsmU4ltlpJWtajgJA6mvzlrbUz2rL85KAIiI8kVpQ5J/ePqef0q03hCEsgu2sqdUpZJPDvk9VGmO0MqW/lWRnehcNvypS2nGMZz1potLDgc/hxzT0pQYZYYbQ0kc9uorqshhWBkEnua6uBMnQo+LlYwrOSK0fRUxx9rwlL4GmyF7A8xv8ArikbUUFy2X6bHebLeH1LSnOfIolSfyIpp9nzxTJKuQWOEAn151W9my+Yl323e8vxLM8Wv/bpU5xuDcBRCcD8lVlzaCcDvWve1maj/wBJx2EPbSJQ4UKGVKCckkenL61l0FoKWCeQphWXyJm2OFtIpw9n98fsclbS0ly3vnLrX7pH7SfXA5dfpQOLELySQkkdKY7TbD90TtleD8KFSaDcFJYZqvlcbS7HWlbLifKtPapWchCQcZAxtSnZZsyK8GY7JERsqS94hyV42BSOh260est5t99ie92t8OI4ilaDsttXVKknkasxluRn21uDCiTUVwhs3CG5GkpJbX+6cEEbgg19AkHFSJO9S0msMWm08oSZek7uy4r3K9OLQeReZBUO3mB/lQqJ7OpC5Xj3GcXlE+Y451ptcAKRDS0weYxHz1Ns1hsE2+0tQ2UNoGQjkSetfFwtiHUjw0pUvGyFbZ+B6UYVgDOM14UggGitphbHbJCoTlB5Riuq9FfaLz0uMsodH40r6EdMdPjVGx6aly7el9vwiiOR47AT51kZ3zzI/vWyXqziejjZKUPp7jyrHZVLbrP2S24iDbpyJZTlXLhPz/Dj0rKnVfT9n2vRq16iMlu9gLUeqIpsaIVsUgrKQjY/X6UI0pZFOLTIdbJcWcpChy9TRC0aRuEycZU5oBKuaAnAHwrRbPZERACU5UR9KvaPTeKOfbKWpuU3x0eWW1iMgcOM8ztzPejiQlpHGshKQMkq2wP5VDJkRbZEclTHUMMNjKlrOAKxTX/tBf1CF2+1FbFsyQtZGFP/ANE+lXuiolk99p+uzqB42q0OZtjZ+8dB/wDkq/8Az+tKEFgJTxq5kcqhjx+I5GaLwIpKxxpISe9LbGIv2KIVHPDkA5psgI4QEkDiJ5DfFR2uKwy1sgqJHSirKQknCUpHx3oSGyYZSMKO49K6pwg4GVAemBXVJAoe1yMy3eLc6hAC32FBZ78CgE/kf0oPZVKjRG5TCih0nhJHLGK6uqtLs2KuYIpa7mSJV6Q0+4VIjspS2OwIyf5fQVUt7aeFI6V1dRPoR/6Hi1xGRHKuAZGf50Zt4A8EgAELQBgcskA/rXV1CEGLcn7xXmO77h/+52rOtHvOxLtdXo61IcE1/cdcLVzrq6mwK1/Rr9lkuTYaXX8cZG5A51YdyBsSPhXV1WCmSjkK+xyrq6uOOFe9RXV1cce4HPrXypIwnIrq6uOPUtoHICo5zyo0N55sDiQkkA8uVeV1EiGfm3U2pbrqSc4u5yVKbaWUtsI2bTjrw9/U1TitpUEkjc866upTGoKwkg8wNqZbYwgjlzya6uoThht6RwZxvnFFY8dpasqTklO9dXUSIZ6SUkgE4B2rq6uqCD//2Q==</t>
-  </si>
-  <si>
-    <t>https://encrypted-tbn0.gstatic.com/images?q=tbn:ANd9GcQ98IZk2hx7LuwyZY1hJyI36EIXu8gGzBit7DX2ZFtlS-KPoaHNmzFi2rJ2C3hzrlUQsuHJrLO8vIwHp_VM_pF3NTp33BHAlDcqcpMqLe8U</t>
+    <t>SUGAR, YES PLEASE</t>
+  </si>
+  <si>
+    <t>IM FEELING FRUITY</t>
+  </si>
+  <si>
+    <t>LOVE YOU SO MATCHA</t>
+  </si>
+  <si>
+    <t>LOVE YOU SO BERRY MATCHA</t>
+  </si>
+  <si>
+    <t>DIY ACAI BOWL</t>
+  </si>
+  <si>
+    <t>Blueberry</t>
+  </si>
+  <si>
+    <t>Dragonfruit</t>
+  </si>
+  <si>
+    <t>Banana</t>
+  </si>
+  <si>
+    <t>Oreo Crush</t>
+  </si>
+  <si>
+    <t>Biscoff Crush</t>
+  </si>
+  <si>
+    <t>Almond Butter</t>
+  </si>
+  <si>
+    <t>Cookie Butter</t>
+  </si>
+  <si>
+    <t>Hershey Sauce</t>
+  </si>
+  <si>
+    <t>Granola</t>
+  </si>
+  <si>
+    <t>Condensed Milk</t>
+  </si>
+  <si>
+    <t>Matcha Granola</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>slug</t>
+  </si>
+  <si>
+    <t>ItsBubblin'!</t>
+  </si>
+  <si>
+    <t>its-bubblin</t>
+  </si>
+  <si>
+    <t>menu-item</t>
+  </si>
+  <si>
+    <t>sugar-yes-please</t>
+  </si>
+  <si>
+    <t>im-feeling-fruity</t>
+  </si>
+  <si>
+    <t>love-you-so-matcha</t>
+  </si>
+  <si>
+    <t>love-you-so-berry-matcha</t>
+  </si>
+  <si>
+    <t>diy-acai</t>
+  </si>
+  <si>
+    <t>Toppings</t>
+  </si>
+  <si>
+    <t>required</t>
+  </si>
+  <si>
+    <t>max_choices</t>
+  </si>
+  <si>
+    <t>Add Ons</t>
+  </si>
+  <si>
+    <t>group_name</t>
+  </si>
+  <si>
+    <t>menu_item_slug</t>
+  </si>
+  <si>
+    <t>extra_cost</t>
+  </si>
+  <si>
+    <t>Peanut Butter</t>
+  </si>
+  <si>
+    <t>Nutella</t>
+  </si>
+  <si>
+    <t>Oreo</t>
+  </si>
+  <si>
+    <t>Hershey Choco</t>
+  </si>
+  <si>
+    <t>Sauce</t>
+  </si>
+  <si>
+    <t>Choco/White Choco Chip</t>
+  </si>
+  <si>
+    <t>Biscoff</t>
+  </si>
+  <si>
+    <t>Acai, Granola, Biscoff, Chocolate Chip, 1 sauce of choice</t>
+  </si>
+  <si>
+    <t>Create your own Acai</t>
+  </si>
+  <si>
+    <t>business_name</t>
+  </si>
+  <si>
+    <t>https://www.cubesnjuliennes.com/wp-content/uploads/2023/04/Acai-Bowl-Recipe.jpg</t>
   </si>
 </sst>
 </file>
@@ -445,69 +553,1258 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B870803C-A700-5B40-B5AF-458A2A9257DE}">
-  <dimension ref="A1:D4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FF8866BA-E47E-F747-A380-D58F4D10A1D9}">
+  <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C39" sqref="C39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B870803C-A700-5B40-B5AF-458A2A9257DE}">
+  <dimension ref="A1:F6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="211" zoomScaleNormal="211" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="25.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="53.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="55.83203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="22.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>46</v>
+      </c>
+      <c r="F1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2">
+        <v>9</v>
+      </c>
+      <c r="C2" t="s">
+        <v>44</v>
+      </c>
+      <c r="D2" t="s">
+        <v>47</v>
+      </c>
+      <c r="E2" t="s">
+        <v>23</v>
+      </c>
+      <c r="F2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3">
+        <v>9</v>
+      </c>
+      <c r="C3" t="s">
+        <v>44</v>
+      </c>
+      <c r="D3" t="s">
+        <v>47</v>
+      </c>
+      <c r="E3" t="s">
+        <v>23</v>
+      </c>
+      <c r="F3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4">
+        <v>9</v>
+      </c>
+      <c r="C4" t="s">
+        <v>44</v>
+      </c>
+      <c r="D4" t="s">
+        <v>47</v>
+      </c>
+      <c r="E4" t="s">
+        <v>23</v>
+      </c>
+      <c r="F4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5">
+        <v>9.5</v>
+      </c>
+      <c r="C5" t="s">
+        <v>44</v>
+      </c>
+      <c r="D5" t="s">
+        <v>47</v>
+      </c>
+      <c r="E5" t="s">
+        <v>23</v>
+      </c>
+      <c r="F5" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6">
+        <v>5.9</v>
+      </c>
+      <c r="C6" t="s">
+        <v>45</v>
+      </c>
+      <c r="D6" t="s">
+        <v>47</v>
+      </c>
+      <c r="E6" t="s">
+        <v>23</v>
+      </c>
+      <c r="F6" t="s">
+        <v>29</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{75D3DD44-EEAE-CA45-9791-400D5C172BCA}">
+  <dimension ref="A1:D10"/>
+  <sheetViews>
+    <sheetView topLeftCell="D1" zoomScale="186" workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="13.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>24</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="C1" t="s">
-        <v>2</v>
+        <v>31</v>
       </c>
       <c r="D1" t="s">
-        <v>9</v>
+        <v>32</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>3</v>
+        <v>29</v>
       </c>
       <c r="B2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2">
-        <v>1.0900000000000001</v>
-      </c>
-      <c r="D2" t="s">
-        <v>10</v>
+        <v>30</v>
+      </c>
+      <c r="C2" t="b">
+        <v>1</v>
+      </c>
+      <c r="D2">
+        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>5</v>
+        <v>25</v>
       </c>
       <c r="B3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3">
-        <v>1.6</v>
-      </c>
-      <c r="D3" t="s">
-        <v>12</v>
+        <v>33</v>
+      </c>
+      <c r="C3" t="b">
+        <v>0</v>
+      </c>
+      <c r="D3">
+        <v>99</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>7</v>
+        <v>26</v>
       </c>
       <c r="B4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4">
-        <v>2.2000000000000002</v>
-      </c>
-      <c r="D4" t="s">
+        <v>33</v>
+      </c>
+      <c r="C4" t="b">
+        <v>0</v>
+      </c>
+      <c r="D4">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>27</v>
+      </c>
+      <c r="B5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C5" t="b">
+        <v>0</v>
+      </c>
+      <c r="D5">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>28</v>
+      </c>
+      <c r="B6" t="s">
+        <v>33</v>
+      </c>
+      <c r="C6" t="b">
+        <v>0</v>
+      </c>
+      <c r="D6">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>25</v>
+      </c>
+      <c r="B7" t="s">
+        <v>41</v>
+      </c>
+      <c r="C7" t="b">
+        <v>1</v>
+      </c>
+      <c r="D7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>26</v>
+      </c>
+      <c r="B8" t="s">
+        <v>41</v>
+      </c>
+      <c r="C8" t="b">
+        <v>1</v>
+      </c>
+      <c r="D8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>27</v>
+      </c>
+      <c r="B9" t="s">
+        <v>41</v>
+      </c>
+      <c r="C9" t="b">
+        <v>1</v>
+      </c>
+      <c r="D9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>28</v>
+      </c>
+      <c r="B10" t="s">
+        <v>41</v>
+      </c>
+      <c r="C10" t="b">
+        <v>1</v>
+      </c>
+      <c r="D10">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7B61E871-18E0-0640-91EC-1BE01419B288}">
+  <dimension ref="A1:D65"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B71" sqref="B71"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="22.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.83203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>30</v>
+      </c>
+      <c r="B4" t="s">
+        <v>29</v>
+      </c>
+      <c r="C4" t="s">
         <v>11</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>30</v>
+      </c>
+      <c r="B5" t="s">
+        <v>29</v>
+      </c>
+      <c r="C5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>30</v>
+      </c>
+      <c r="B6" t="s">
+        <v>29</v>
+      </c>
+      <c r="C6" t="s">
+        <v>13</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>30</v>
+      </c>
+      <c r="B7" t="s">
+        <v>29</v>
+      </c>
+      <c r="C7" t="s">
+        <v>14</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>30</v>
+      </c>
+      <c r="B8" t="s">
+        <v>29</v>
+      </c>
+      <c r="C8" t="s">
+        <v>15</v>
+      </c>
+      <c r="D8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>30</v>
+      </c>
+      <c r="B9" t="s">
+        <v>29</v>
+      </c>
+      <c r="C9" t="s">
+        <v>16</v>
+      </c>
+      <c r="D9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>30</v>
+      </c>
+      <c r="B10" t="s">
+        <v>29</v>
+      </c>
+      <c r="C10" t="s">
+        <v>42</v>
+      </c>
+      <c r="D10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>30</v>
+      </c>
+      <c r="B11" t="s">
+        <v>29</v>
+      </c>
+      <c r="C11" t="s">
+        <v>17</v>
+      </c>
+      <c r="D11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>30</v>
+      </c>
+      <c r="B12" t="s">
+        <v>29</v>
+      </c>
+      <c r="C12" t="s">
+        <v>18</v>
+      </c>
+      <c r="D12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>30</v>
+      </c>
+      <c r="B13" t="s">
+        <v>29</v>
+      </c>
+      <c r="C13" t="s">
+        <v>19</v>
+      </c>
+      <c r="D13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>41</v>
+      </c>
+      <c r="B14" t="s">
+        <v>25</v>
+      </c>
+      <c r="C14" t="s">
+        <v>15</v>
+      </c>
+      <c r="D14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>41</v>
+      </c>
+      <c r="B15" t="s">
+        <v>25</v>
+      </c>
+      <c r="C15" t="s">
+        <v>14</v>
+      </c>
+      <c r="D15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>41</v>
+      </c>
+      <c r="B16" t="s">
+        <v>25</v>
+      </c>
+      <c r="C16" t="s">
+        <v>37</v>
+      </c>
+      <c r="D16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>41</v>
+      </c>
+      <c r="B17" t="s">
+        <v>25</v>
+      </c>
+      <c r="C17" t="s">
+        <v>38</v>
+      </c>
+      <c r="D17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>41</v>
+      </c>
+      <c r="B18" t="s">
+        <v>25</v>
+      </c>
+      <c r="C18" t="s">
+        <v>40</v>
+      </c>
+      <c r="D18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>33</v>
+      </c>
+      <c r="B19" t="s">
+        <v>25</v>
+      </c>
+      <c r="C19" t="s">
+        <v>15</v>
+      </c>
+      <c r="D19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>33</v>
+      </c>
+      <c r="B20" t="s">
+        <v>25</v>
+      </c>
+      <c r="C20" t="s">
+        <v>14</v>
+      </c>
+      <c r="D20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>33</v>
+      </c>
+      <c r="B21" t="s">
+        <v>25</v>
+      </c>
+      <c r="C21" t="s">
+        <v>37</v>
+      </c>
+      <c r="D21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>33</v>
+      </c>
+      <c r="B22" t="s">
+        <v>25</v>
+      </c>
+      <c r="C22" t="s">
+        <v>38</v>
+      </c>
+      <c r="D22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>33</v>
+      </c>
+      <c r="B23" t="s">
+        <v>25</v>
+      </c>
+      <c r="C23" t="s">
+        <v>40</v>
+      </c>
+      <c r="D23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>33</v>
+      </c>
+      <c r="B24" t="s">
+        <v>25</v>
+      </c>
+      <c r="C24" t="s">
+        <v>39</v>
+      </c>
+      <c r="D24">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>33</v>
+      </c>
+      <c r="B25" t="s">
+        <v>25</v>
+      </c>
+      <c r="C25" t="s">
+        <v>43</v>
+      </c>
+      <c r="D25">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>33</v>
+      </c>
+      <c r="B26" t="s">
+        <v>25</v>
+      </c>
+      <c r="C26" t="s">
+        <v>17</v>
+      </c>
+      <c r="D26">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>41</v>
+      </c>
+      <c r="B27" t="s">
+        <v>26</v>
+      </c>
+      <c r="C27" t="s">
+        <v>15</v>
+      </c>
+      <c r="D27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>41</v>
+      </c>
+      <c r="B28" t="s">
+        <v>26</v>
+      </c>
+      <c r="C28" t="s">
+        <v>14</v>
+      </c>
+      <c r="D28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>41</v>
+      </c>
+      <c r="B29" t="s">
+        <v>26</v>
+      </c>
+      <c r="C29" t="s">
+        <v>37</v>
+      </c>
+      <c r="D29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>41</v>
+      </c>
+      <c r="B30" t="s">
+        <v>26</v>
+      </c>
+      <c r="C30" t="s">
+        <v>38</v>
+      </c>
+      <c r="D30">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>41</v>
+      </c>
+      <c r="B31" t="s">
+        <v>26</v>
+      </c>
+      <c r="C31" t="s">
+        <v>40</v>
+      </c>
+      <c r="D31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>33</v>
+      </c>
+      <c r="B32" t="s">
+        <v>26</v>
+      </c>
+      <c r="C32" t="s">
+        <v>15</v>
+      </c>
+      <c r="D32">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>33</v>
+      </c>
+      <c r="B33" t="s">
+        <v>26</v>
+      </c>
+      <c r="C33" t="s">
+        <v>14</v>
+      </c>
+      <c r="D33">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>33</v>
+      </c>
+      <c r="B34" t="s">
+        <v>26</v>
+      </c>
+      <c r="C34" t="s">
+        <v>37</v>
+      </c>
+      <c r="D34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>33</v>
+      </c>
+      <c r="B35" t="s">
+        <v>26</v>
+      </c>
+      <c r="C35" t="s">
+        <v>38</v>
+      </c>
+      <c r="D35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>33</v>
+      </c>
+      <c r="B36" t="s">
+        <v>26</v>
+      </c>
+      <c r="C36" t="s">
+        <v>40</v>
+      </c>
+      <c r="D36">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>33</v>
+      </c>
+      <c r="B37" t="s">
+        <v>26</v>
+      </c>
+      <c r="C37" t="s">
+        <v>39</v>
+      </c>
+      <c r="D37">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>33</v>
+      </c>
+      <c r="B38" t="s">
+        <v>26</v>
+      </c>
+      <c r="C38" t="s">
+        <v>43</v>
+      </c>
+      <c r="D38">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>33</v>
+      </c>
+      <c r="B39" t="s">
+        <v>26</v>
+      </c>
+      <c r="C39" t="s">
+        <v>17</v>
+      </c>
+      <c r="D39">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>41</v>
+      </c>
+      <c r="B40" t="s">
+        <v>27</v>
+      </c>
+      <c r="C40" t="s">
+        <v>15</v>
+      </c>
+      <c r="D40">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>41</v>
+      </c>
+      <c r="B41" t="s">
+        <v>27</v>
+      </c>
+      <c r="C41" t="s">
+        <v>14</v>
+      </c>
+      <c r="D41">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
+        <v>41</v>
+      </c>
+      <c r="B42" t="s">
+        <v>27</v>
+      </c>
+      <c r="C42" t="s">
+        <v>37</v>
+      </c>
+      <c r="D42">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
+        <v>41</v>
+      </c>
+      <c r="B43" t="s">
+        <v>27</v>
+      </c>
+      <c r="C43" t="s">
+        <v>38</v>
+      </c>
+      <c r="D43">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
+        <v>41</v>
+      </c>
+      <c r="B44" t="s">
+        <v>27</v>
+      </c>
+      <c r="C44" t="s">
+        <v>40</v>
+      </c>
+      <c r="D44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
+        <v>33</v>
+      </c>
+      <c r="B45" t="s">
+        <v>27</v>
+      </c>
+      <c r="C45" t="s">
+        <v>15</v>
+      </c>
+      <c r="D45">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
+        <v>33</v>
+      </c>
+      <c r="B46" t="s">
+        <v>27</v>
+      </c>
+      <c r="C46" t="s">
+        <v>14</v>
+      </c>
+      <c r="D46">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A47" t="s">
+        <v>33</v>
+      </c>
+      <c r="B47" t="s">
+        <v>27</v>
+      </c>
+      <c r="C47" t="s">
+        <v>37</v>
+      </c>
+      <c r="D47">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A48" t="s">
+        <v>33</v>
+      </c>
+      <c r="B48" t="s">
+        <v>27</v>
+      </c>
+      <c r="C48" t="s">
+        <v>38</v>
+      </c>
+      <c r="D48">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A49" t="s">
+        <v>33</v>
+      </c>
+      <c r="B49" t="s">
+        <v>27</v>
+      </c>
+      <c r="C49" t="s">
+        <v>40</v>
+      </c>
+      <c r="D49">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A50" t="s">
+        <v>33</v>
+      </c>
+      <c r="B50" t="s">
+        <v>27</v>
+      </c>
+      <c r="C50" t="s">
+        <v>39</v>
+      </c>
+      <c r="D50">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A51" t="s">
+        <v>33</v>
+      </c>
+      <c r="B51" t="s">
+        <v>27</v>
+      </c>
+      <c r="C51" t="s">
+        <v>43</v>
+      </c>
+      <c r="D51">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A52" t="s">
+        <v>33</v>
+      </c>
+      <c r="B52" t="s">
+        <v>27</v>
+      </c>
+      <c r="C52" t="s">
+        <v>17</v>
+      </c>
+      <c r="D52">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A53" t="s">
+        <v>41</v>
+      </c>
+      <c r="B53" t="s">
+        <v>28</v>
+      </c>
+      <c r="C53" t="s">
+        <v>15</v>
+      </c>
+      <c r="D53">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A54" t="s">
+        <v>41</v>
+      </c>
+      <c r="B54" t="s">
+        <v>28</v>
+      </c>
+      <c r="C54" t="s">
+        <v>14</v>
+      </c>
+      <c r="D54">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A55" t="s">
+        <v>41</v>
+      </c>
+      <c r="B55" t="s">
+        <v>28</v>
+      </c>
+      <c r="C55" t="s">
+        <v>37</v>
+      </c>
+      <c r="D55">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A56" t="s">
+        <v>41</v>
+      </c>
+      <c r="B56" t="s">
+        <v>28</v>
+      </c>
+      <c r="C56" t="s">
+        <v>38</v>
+      </c>
+      <c r="D56">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A57" t="s">
+        <v>41</v>
+      </c>
+      <c r="B57" t="s">
+        <v>28</v>
+      </c>
+      <c r="C57" t="s">
+        <v>40</v>
+      </c>
+      <c r="D57">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A58" t="s">
+        <v>33</v>
+      </c>
+      <c r="B58" t="s">
+        <v>28</v>
+      </c>
+      <c r="C58" t="s">
+        <v>15</v>
+      </c>
+      <c r="D58">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A59" t="s">
+        <v>33</v>
+      </c>
+      <c r="B59" t="s">
+        <v>28</v>
+      </c>
+      <c r="C59" t="s">
+        <v>14</v>
+      </c>
+      <c r="D59">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A60" t="s">
+        <v>33</v>
+      </c>
+      <c r="B60" t="s">
+        <v>28</v>
+      </c>
+      <c r="C60" t="s">
+        <v>37</v>
+      </c>
+      <c r="D60">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A61" t="s">
+        <v>33</v>
+      </c>
+      <c r="B61" t="s">
+        <v>28</v>
+      </c>
+      <c r="C61" t="s">
+        <v>38</v>
+      </c>
+      <c r="D61">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A62" t="s">
+        <v>33</v>
+      </c>
+      <c r="B62" t="s">
+        <v>28</v>
+      </c>
+      <c r="C62" t="s">
+        <v>40</v>
+      </c>
+      <c r="D62">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A63" t="s">
+        <v>33</v>
+      </c>
+      <c r="B63" t="s">
+        <v>28</v>
+      </c>
+      <c r="C63" t="s">
+        <v>39</v>
+      </c>
+      <c r="D63">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A64" t="s">
+        <v>33</v>
+      </c>
+      <c r="B64" t="s">
+        <v>28</v>
+      </c>
+      <c r="C64" t="s">
+        <v>43</v>
+      </c>
+      <c r="D64">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A65" t="s">
+        <v>33</v>
+      </c>
+      <c r="B65" t="s">
+        <v>28</v>
+      </c>
+      <c r="C65" t="s">
+        <v>17</v>
+      </c>
+      <c r="D65">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>